<commit_message>
5/17 oh no I find a bug after meeting.
</commit_message>
<xml_diff>
--- a/nsf/波長vs能源消耗.xlsx
+++ b/nsf/波長vs能源消耗.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="5265"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7635" windowHeight="4770"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>W</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -65,13 +65,78 @@
     <t>sql=2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>40</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>50</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>60</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sql=2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sql=1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>49:30:00 AM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>power</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>energy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>capacity</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>32:04:00 AM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="176" formatCode="0.000_ "/>
+    <numFmt numFmtId="180" formatCode="0.000_);[Red]\(0.000\)"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -112,7 +177,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -123,6 +188,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -375,11 +449,11 @@
         </c:hiLowLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="236737168"/>
-        <c:axId val="236737728"/>
+        <c:axId val="240109040"/>
+        <c:axId val="240109600"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="236737168"/>
+        <c:axId val="240109040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -483,7 +557,7 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="236737728"/>
+        <c:crossAx val="240109600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -491,7 +565,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="236737728"/>
+        <c:axId val="240109600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="643.50000000000011"/>
@@ -603,7 +677,7 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="236737168"/>
+        <c:crossAx val="240109040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.1"/>
@@ -930,11 +1004,11 @@
         </c:hiLowLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="236739968"/>
-        <c:axId val="236740528"/>
+        <c:axId val="240111840"/>
+        <c:axId val="240112400"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="236739968"/>
+        <c:axId val="240111840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1038,7 +1112,7 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="236740528"/>
+        <c:crossAx val="240112400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -1046,7 +1120,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="236740528"/>
+        <c:axId val="240112400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="691"/>
@@ -1159,7 +1233,7 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="236739968"/>
+        <c:crossAx val="240111840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -2654,10 +2728,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q11"/>
+  <dimension ref="A1:AA11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AA6" sqref="AA6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -2665,10 +2739,16 @@
     <col min="3" max="3" width="9.5" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.5" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9" style="4"/>
     <col min="15" max="15" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.25" customWidth="1"/>
+    <col min="21" max="21" width="10" style="2" customWidth="1"/>
+    <col min="23" max="23" width="9" style="4"/>
+    <col min="24" max="26" width="9" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -2699,8 +2779,26 @@
       <c r="K1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>19</v>
+      </c>
+      <c r="S1" t="s">
+        <v>20</v>
+      </c>
+      <c r="T1" t="s">
+        <v>21</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>5</v>
       </c>
@@ -2725,20 +2823,38 @@
       <c r="K2" s="1">
         <v>67.581299999999999</v>
       </c>
-      <c r="N2" s="3">
-        <v>685.93650000000002</v>
-      </c>
-      <c r="O2" s="3">
-        <v>1552.837</v>
-      </c>
-      <c r="P2" s="3">
-        <v>68.533180000000002</v>
-      </c>
-      <c r="Q2" s="2">
-        <v>0.80833333333333324</v>
+      <c r="Q2" s="4">
+        <v>10</v>
+      </c>
+      <c r="R2" s="3">
+        <v>688.52300000000002</v>
+      </c>
+      <c r="S2" s="3">
+        <v>1583.876</v>
+      </c>
+      <c r="T2" s="3">
+        <v>60</v>
+      </c>
+      <c r="U2" s="2">
+        <v>0.62013888888888891</v>
+      </c>
+      <c r="W2" s="4">
+        <v>5</v>
+      </c>
+      <c r="X2" s="5">
+        <v>644.11199999999997</v>
+      </c>
+      <c r="Y2" s="5">
+        <v>855.47199999999998</v>
+      </c>
+      <c r="Z2" s="5">
+        <v>33</v>
+      </c>
+      <c r="AA2" s="2">
+        <v>2.0833333333333333E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>8</v>
       </c>
@@ -2763,17 +2879,38 @@
       <c r="K3" s="1">
         <v>97.836020000000005</v>
       </c>
-      <c r="N3" s="3">
-        <v>688.52300000000002</v>
-      </c>
-      <c r="O3" s="3">
-        <v>1583.876</v>
-      </c>
-      <c r="P3" s="3">
-        <v>78.5</v>
+      <c r="Q3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="R3" s="3">
+        <v>686.76599999999996</v>
+      </c>
+      <c r="S3" s="3">
+        <v>1562.7919999999999</v>
+      </c>
+      <c r="T3" s="3">
+        <v>109.97969999999999</v>
+      </c>
+      <c r="U3" s="2">
+        <v>0.44861111111111113</v>
+      </c>
+      <c r="W3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="X3" s="5">
+        <v>643.62599999999998</v>
+      </c>
+      <c r="Y3" s="5">
+        <v>872.55600000000004</v>
+      </c>
+      <c r="Z3" s="5">
+        <v>38.00215</v>
+      </c>
+      <c r="AA3" s="2">
+        <v>9.7222222222222224E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>10</v>
       </c>
@@ -2798,8 +2935,26 @@
       <c r="K4" s="1">
         <v>128.4853</v>
       </c>
+      <c r="Q4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="R4" s="3">
+        <v>686.76599999999996</v>
+      </c>
+      <c r="S4" s="3">
+        <v>1562.7919999999999</v>
+      </c>
+      <c r="T4" s="3">
+        <v>155</v>
+      </c>
+      <c r="U4" s="2">
+        <v>0.24305555555555555</v>
+      </c>
+      <c r="W4" s="4" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>20</v>
       </c>
@@ -2824,8 +2979,38 @@
       <c r="K5" s="1">
         <v>165.2176</v>
       </c>
+      <c r="Q5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="R5" s="3">
+        <v>686.76599999999996</v>
+      </c>
+      <c r="S5" s="3">
+        <v>1562.7919999999999</v>
+      </c>
+      <c r="T5" s="3">
+        <v>209.25</v>
+      </c>
+      <c r="U5" s="2">
+        <v>0.19652777777777777</v>
+      </c>
+      <c r="W5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="X5" s="5">
+        <v>643.62599999999998</v>
+      </c>
+      <c r="Y5" s="5">
+        <v>872.55600000000004</v>
+      </c>
+      <c r="Z5" s="5">
+        <v>46</v>
+      </c>
+      <c r="AA5" s="6">
+        <v>8.7280092592592604E-2</v>
+      </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>30</v>
       </c>
@@ -2850,8 +3035,26 @@
       <c r="K6" s="1">
         <v>180.5</v>
       </c>
+      <c r="Q6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="R6" s="3">
+        <v>688.52300000000002</v>
+      </c>
+      <c r="S6" s="3">
+        <v>1583.876</v>
+      </c>
+      <c r="T6" s="3">
+        <v>245</v>
+      </c>
+      <c r="U6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="W6" s="4" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>40</v>
       </c>
@@ -2876,8 +3079,23 @@
       <c r="K7" s="1">
         <v>219.2166</v>
       </c>
+      <c r="Q7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="R7" s="3">
+        <v>688.52300000000002</v>
+      </c>
+      <c r="S7" s="3">
+        <v>1583.876</v>
+      </c>
+      <c r="T7" s="3">
+        <v>200.5</v>
+      </c>
+      <c r="U7" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="H8">
         <v>70</v>
       </c>
@@ -2891,7 +3109,7 @@
         <v>263.1927</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="H9">
         <v>80</v>
       </c>
@@ -2905,7 +3123,7 @@
         <v>283.73680000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="H10">
         <v>90</v>
       </c>
@@ -2919,7 +3137,7 @@
         <v>365.94150000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="H11">
         <v>100</v>
       </c>

</xml_diff>